<commit_message>
Ya está testeada la ALU con el ALUControl, no sintetiza porque hay algun problema con el archivo registers.v, ya veo si puedo solucionarlo
</commit_message>
<xml_diff>
--- a/Documentos para el TP final/Tabla de instrucciones.xlsx
+++ b/Documentos para el TP final/Tabla de instrucciones.xlsx
@@ -944,7 +944,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,6 +972,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1048,17 +1060,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1067,12 +1073,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1097,55 +1097,90 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,11 +1483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -1471,7 +1506,7 @@
     <col min="13" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1509,1365 +1544,1366 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.15">
+      <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="M2" s="45"/>
+    </row>
+    <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A3" s="35"/>
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="M3" s="45"/>
+    </row>
+    <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A4" s="35"/>
+      <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="M4" s="45"/>
+    </row>
+    <row r="5" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="35"/>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="M5" s="34"/>
+    </row>
+    <row r="6" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="35"/>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="35"/>
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="35"/>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A9" s="35"/>
+      <c r="B9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.15">
+      <c r="A10" s="35"/>
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="35"/>
+      <c r="B11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="27" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" s="35"/>
+      <c r="B12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="27" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" s="35"/>
+      <c r="B13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A14" s="35"/>
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A15" s="35"/>
+      <c r="B15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="27" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A16" s="35"/>
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>129</v>
       </c>
+      <c r="M16" s="34"/>
     </row>
     <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="E17" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="31" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="18"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="24" t="s">
+      <c r="E19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25" t="s">
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="K19" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="18" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="8" t="s">
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28" t="s">
+      <c r="A21" s="38"/>
+      <c r="B21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="29" t="s">
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="8" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="29" t="s">
+      <c r="E22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="8" t="s">
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="29" t="s">
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="8" t="s">
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="29" t="s">
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="8" t="s">
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28" t="s">
+      <c r="A25" s="38"/>
+      <c r="B25" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="29" t="s">
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="8" t="s">
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="8" t="s">
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="38"/>
+      <c r="B27" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="29" t="s">
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="8" t="s">
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="5" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="36" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="29" t="s">
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="8" t="s">
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="29" t="s">
+      <c r="E29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="8" t="s">
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="L29" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="29" t="s">
+      <c r="E30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="8" t="s">
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="K30" s="8" t="s">
+      <c r="K30" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="L30" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="38"/>
+      <c r="B31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="29" t="s">
+      <c r="E31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="8" t="s">
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="K31" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="29" t="s">
+      <c r="E32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="8" t="s">
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="5" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28" t="s">
+      <c r="A33" s="38"/>
+      <c r="B33" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="29" t="s">
+      <c r="E33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="8" t="s">
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="J33" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="K33" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="L33" s="6" t="s">
+      <c r="L33" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="36" x14ac:dyDescent="0.15">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28" t="s">
+      <c r="A34" s="38"/>
+      <c r="B34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="29" t="s">
+      <c r="E34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="8" t="s">
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="J34" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="L34" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="38"/>
+      <c r="B35" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="29" t="s">
+      <c r="E35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="8" t="s">
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="L35" s="6" t="s">
+      <c r="L35" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="29" t="s">
+      <c r="E36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="8" t="s">
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K36" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="29" t="s">
+      <c r="E37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="8" t="s">
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="L37" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="63" x14ac:dyDescent="0.15">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="8" t="s">
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="K38" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="L38" s="6" t="s">
+      <c r="L38" s="5" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="63" x14ac:dyDescent="0.15">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="39"/>
+      <c r="B39" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="14" t="s">
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="J39" s="15" t="s">
+      <c r="J39" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="K39" s="14" t="s">
+      <c r="K39" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="L39" s="13" t="s">
+      <c r="L39" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="14"/>
     </row>
     <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="23" t="s">
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="I41" s="25" t="s">
+      <c r="I41" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="J41" s="26" t="s">
+      <c r="J41" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="K41" s="25" t="s">
+      <c r="K41" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="L41" s="23" t="s">
+      <c r="L41" s="18" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="72" x14ac:dyDescent="0.15">
-      <c r="A42" s="35"/>
-      <c r="B42" s="36" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I42" s="37" t="s">
+      <c r="I42" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="J42" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="K42" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="L42" s="6" t="s">
+      <c r="L42" s="5" t="s">
         <v>234</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F35:H35"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="D38:H38"/>
     <mergeCell ref="D39:H39"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="A19:A39"/>
     <mergeCell ref="A41:A42"/>
@@ -2878,6 +2914,12 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F25:H25"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
All R-Type instructions working
</commit_message>
<xml_diff>
--- a/Documentos para el TP final/Tabla de instrucciones.xlsx
+++ b/Documentos para el TP final/Tabla de instrucciones.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Hoja1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="243">
   <si>
     <t>Instrucción</t>
   </si>
@@ -552,9 +552,6 @@
     <t>NOR rd, rs, rt</t>
   </si>
   <si>
-    <t>rd &lt;- rs NXOR rt</t>
-  </si>
-  <si>
     <t>NOR 2, 15, 5</t>
   </si>
   <si>
@@ -901,13 +898,25 @@
   </si>
   <si>
     <t>000000-00101-000000000000000-001000</t>
+  </si>
+  <si>
+    <t>rd &lt;- rs NOR rt</t>
+  </si>
+  <si>
+    <t>Tested</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Not included</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,6 +948,21 @@
     <font>
       <sz val="6.5"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="6.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6.5"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -977,13 +1001,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1052,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1074,6 +1098,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1123,8 +1150,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1135,19 +1162,12 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1175,12 +1195,26 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1485,9 +1519,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -1502,8 +1536,9 @@
     <col min="9" max="9" width="12.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="12" max="12" width="25.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1529,7 +1564,7 @@
         <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>50</v>
@@ -1543,903 +1578,961 @@
       <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.15">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="35"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="45"/>
+      <c r="M3" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="35"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="45"/>
+      <c r="M4" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="35"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="34"/>
+      <c r="M5" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="35"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="35"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="E7" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="28" t="s">
         <v>85</v>
       </c>
+      <c r="M7" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="35"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="E8" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="34"/>
+      <c r="M8" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="35"/>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="27" t="s">
+      <c r="E9" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="31" t="s">
         <v>85</v>
       </c>
+      <c r="M9" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A10" s="35"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="28" t="s">
         <v>100</v>
       </c>
+      <c r="M10" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="35"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="27" t="s">
+      <c r="E11" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="31" t="s">
         <v>105</v>
       </c>
+      <c r="M11" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="35"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="27" t="s">
+      <c r="E12" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="31" t="s">
         <v>110</v>
       </c>
+      <c r="M12" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="35"/>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="27" t="s">
+      <c r="E13" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="31" t="s">
         <v>115</v>
       </c>
+      <c r="M13" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="35"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="27" t="s">
+      <c r="E14" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="31" t="s">
         <v>120</v>
       </c>
+      <c r="M14" s="29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="35"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="27" t="s">
+      <c r="E15" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="L15" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="L15" s="27" t="s">
-        <v>125</v>
+      <c r="M15" s="29" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A16" s="35"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="E16" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="K16" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="L16" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A17" s="34"/>
+      <c r="B17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="J17" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="M16" s="34"/>
-    </row>
-    <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="36"/>
-      <c r="B17" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="I17" s="32" t="s">
+      <c r="K17" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="K17" s="32" t="s">
+      <c r="L17" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="31" t="s">
+      <c r="M17" s="48" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A19" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A19" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="42" t="s">
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="K19" s="19" t="s">
+      <c r="J19" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
-      <c r="B20" s="21" t="s">
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A20" s="36"/>
+      <c r="B20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="K20" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="L20" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="38"/>
-      <c r="B21" s="21" t="s">
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A21" s="36"/>
+      <c r="B21" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="6" t="s">
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="J21" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="K21" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="L21" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="38"/>
-      <c r="B22" s="21" t="s">
+      <c r="M21" s="29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A22" s="36"/>
+      <c r="B22" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>121</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
       <c r="I22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="K22" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="38"/>
-      <c r="B23" s="21" t="s">
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A23" s="36"/>
+      <c r="B23" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
       <c r="I23" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A24" s="38"/>
-      <c r="B24" s="21" t="s">
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A24" s="36"/>
+      <c r="B24" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
       <c r="I24" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K24" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="38"/>
-      <c r="B25" s="21" t="s">
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="36"/>
+      <c r="B25" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="J25" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A26" s="36"/>
+      <c r="B26" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
-      <c r="B26" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="J26" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A27" s="36"/>
+      <c r="B27" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="L26" s="5" t="s">
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="29" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A27" s="38"/>
-      <c r="B27" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="6" t="s">
+      <c r="J27" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="K27" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="L27" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="36" x14ac:dyDescent="0.15">
+      <c r="A28" s="36"/>
+      <c r="B28" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="36" x14ac:dyDescent="0.15">
-      <c r="A28" s="38"/>
-      <c r="B28" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>71</v>
@@ -2447,31 +2540,32 @@
       <c r="E28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="43" t="s">
+      <c r="F28" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="K28" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="36"/>
+      <c r="B29" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="38"/>
-      <c r="B29" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>71</v>
@@ -2479,31 +2573,32 @@
       <c r="E29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="6" t="s">
-        <v>179</v>
-      </c>
       <c r="J29" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A30" s="36"/>
+      <c r="B30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="38"/>
-      <c r="B30" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>71</v>
@@ -2511,31 +2606,32 @@
       <c r="E30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
+      <c r="F30" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
       <c r="I30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="K30" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="L30" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A31" s="36"/>
+      <c r="B31" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A31" s="38"/>
-      <c r="B31" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>71</v>
@@ -2543,31 +2639,32 @@
       <c r="E31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
+      <c r="F31" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
       <c r="I31" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="K31" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="L31" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A32" s="36"/>
+      <c r="B32" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="38"/>
-      <c r="B32" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>71</v>
@@ -2575,31 +2672,32 @@
       <c r="E32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
+      <c r="F32" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
       <c r="I32" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="J32" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="K32" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="L32" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.15">
+      <c r="A33" s="36"/>
+      <c r="B33" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A33" s="38"/>
-      <c r="B33" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>46</v>
@@ -2607,31 +2705,32 @@
       <c r="E33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
+      <c r="F33" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
       <c r="I33" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J33" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="K33" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="L33" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="1:13" ht="36" x14ac:dyDescent="0.15">
+      <c r="A34" s="36"/>
+      <c r="B34" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="36" x14ac:dyDescent="0.15">
-      <c r="A34" s="38"/>
-      <c r="B34" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>71</v>
@@ -2639,31 +2738,32 @@
       <c r="E34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
+      <c r="F34" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
       <c r="I34" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="K34" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="L34" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.15">
+      <c r="A35" s="36"/>
+      <c r="B35" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A35" s="38"/>
-      <c r="B35" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>71</v>
@@ -2671,27 +2771,28 @@
       <c r="E35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
+      <c r="F35" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
       <c r="I35" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="K35" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="L35" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A36" s="38"/>
-      <c r="B36" s="21" t="s">
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.15">
+      <c r="A36" s="36"/>
+      <c r="B36" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -2703,31 +2804,32 @@
       <c r="E36" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
+      <c r="F36" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
       <c r="I36" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="K36" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="L36" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.15">
+      <c r="A37" s="36"/>
+      <c r="B37" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.15">
-      <c r="A37" s="38"/>
-      <c r="B37" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>71</v>
@@ -2735,131 +2837,136 @@
       <c r="E37" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
+      <c r="F37" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
       <c r="I37" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="J37" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="J37" s="8" t="s">
-        <v>221</v>
-      </c>
       <c r="K37" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="63" x14ac:dyDescent="0.15">
-      <c r="A38" s="38"/>
-      <c r="B38" s="21" t="s">
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.15">
+      <c r="A38" s="36"/>
+      <c r="B38" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="6" t="s">
+      <c r="J38" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="J38" s="7" t="s">
+      <c r="K38" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="K38" s="6" t="s">
+      <c r="L38" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" ht="63" x14ac:dyDescent="0.15">
+      <c r="A39" s="37"/>
+      <c r="B39" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="11" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="63" x14ac:dyDescent="0.15">
-      <c r="A39" s="39"/>
-      <c r="B39" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="10" t="s">
+      <c r="J39" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="K39" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="J39" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="K39" s="10" t="s">
+      <c r="L39" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="L39" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="14"/>
-    </row>
-    <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A41" s="40" t="s">
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A41" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="I41" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="I41" s="19" t="s">
+      <c r="J41" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="K41" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="L41" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="L41" s="18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="72" x14ac:dyDescent="0.15">
-      <c r="A42" s="41"/>
-      <c r="B42" s="24" t="s">
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="1:13" ht="72" x14ac:dyDescent="0.15">
+      <c r="A42" s="39"/>
+      <c r="B42" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2878,20 +2985,21 @@
         <v>46</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I42" s="25" t="s">
-        <v>230</v>
+        <v>182</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>229</v>
       </c>
       <c r="J42" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="K42" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="L42" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>234</v>
-      </c>
+      <c r="M42" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>

<commit_message>
All instructions but jump ones are working. Ready for simulation, changes needed for board use.
</commit_message>
<xml_diff>
--- a/Documentos para el TP final/Tabla de instrucciones.xlsx
+++ b/Documentos para el TP final/Tabla de instrucciones.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="243">
   <si>
     <t>Instrucción</t>
   </si>
@@ -1076,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1101,9 +1101,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,9 +1162,46 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1189,31 +1223,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1517,11 +1542,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -1583,1232 +1608,1269 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="45" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="33"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="33"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="31" t="s">
+      <c r="L4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="33"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="33"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="33"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="33"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="31" t="s">
+      <c r="E8" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="33"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="31" t="s">
+      <c r="E9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A10" s="33"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="33"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="31" t="s">
+      <c r="E11" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="33"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="31" t="s">
+      <c r="E12" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="33"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="I13" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="33"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="31" t="s">
+      <c r="E14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="33"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="31" t="s">
+      <c r="E15" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A16" s="33"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="31" t="s">
+      <c r="E16" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A17" s="46"/>
       <c r="B17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="45" t="s">
+      <c r="E17" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="I17" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="K17" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="45" t="s">
+      <c r="L17" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="48" t="s">
+      <c r="M17" s="35" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="27"/>
-    </row>
-    <row r="19" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A19" s="35" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A19" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="40" t="s">
+      <c r="E19" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="20" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="36"/>
-      <c r="B20" s="22" t="s">
+      <c r="M19" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N19" s="43"/>
+    </row>
+    <row r="20" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A20" s="48"/>
+      <c r="B20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="6" t="s">
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="36"/>
-      <c r="B21" s="22" t="s">
+      <c r="M20" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N20" s="43"/>
+    </row>
+    <row r="21" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A21" s="48"/>
+      <c r="B21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="42" t="s">
+      <c r="E21" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="29" t="s">
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K21" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="L21" s="28" t="s">
+      <c r="L21" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="M21" s="29" t="s">
+      <c r="M21" s="28" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="36"/>
-      <c r="B22" s="22" t="s">
+      <c r="N21" s="43"/>
+    </row>
+    <row r="22" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A22" s="48"/>
+      <c r="B22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="41" t="s">
+      <c r="E22" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="6" t="s">
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="36"/>
-      <c r="B23" s="22" t="s">
+      <c r="M22" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="N22" s="43"/>
+    </row>
+    <row r="23" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A23" s="48"/>
+      <c r="B23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="41" t="s">
+      <c r="E23" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="6" t="s">
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A24" s="36"/>
-      <c r="B24" s="22" t="s">
+      <c r="M23" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N23" s="43"/>
+    </row>
+    <row r="24" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A24" s="48"/>
+      <c r="B24" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="41" t="s">
+      <c r="E24" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="6" t="s">
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="36"/>
-      <c r="B25" s="22" t="s">
+      <c r="M24" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" s="43"/>
+    </row>
+    <row r="25" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="48"/>
+      <c r="B25" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="41" t="s">
+      <c r="E25" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="6" t="s">
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="36"/>
-      <c r="B26" s="22" t="s">
+      <c r="M25" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N25" s="44"/>
+    </row>
+    <row r="26" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A26" s="48"/>
+      <c r="B26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="41" t="s">
+      <c r="E26" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="6" t="s">
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A27" s="36"/>
-      <c r="B27" s="22" t="s">
+      <c r="M26" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A27" s="48"/>
+      <c r="B27" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="42" t="s">
+      <c r="E27" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="29" t="s">
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="L27" s="28" t="s">
+      <c r="L27" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="36" x14ac:dyDescent="0.15">
-      <c r="A28" s="36"/>
-      <c r="B28" s="22" t="s">
+    <row r="28" spans="1:14" ht="36" x14ac:dyDescent="0.15">
+      <c r="A28" s="48"/>
+      <c r="B28" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="41" t="s">
+      <c r="E28" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="6" t="s">
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J28" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="36"/>
-      <c r="B29" s="22" t="s">
+      <c r="M28" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="48"/>
+      <c r="B29" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="41" t="s">
+      <c r="E29" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="6" t="s">
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="36"/>
-      <c r="B30" s="22" t="s">
+      <c r="M29" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A30" s="48"/>
+      <c r="B30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="41" t="s">
+      <c r="E30" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="6" t="s">
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J30" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A31" s="36"/>
-      <c r="B31" s="22" t="s">
+      <c r="M30" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A31" s="48"/>
+      <c r="B31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="41" t="s">
+      <c r="E31" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="6" t="s">
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="K31" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L31" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="36"/>
-      <c r="B32" s="22" t="s">
+      <c r="M31" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A32" s="48"/>
+      <c r="B32" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="6" t="s">
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J32" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="L32" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="M32" s="6"/>
+      <c r="M32" s="28" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.15">
-      <c r="A33" s="36"/>
-      <c r="B33" s="22" t="s">
+      <c r="A33" s="48"/>
+      <c r="B33" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="41" t="s">
+      <c r="E33" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="6" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="J33" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="K33" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L33" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="M33" s="6"/>
+      <c r="M33" s="28" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="36" x14ac:dyDescent="0.15">
-      <c r="A34" s="36"/>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="48"/>
+      <c r="B34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="41" t="s">
+      <c r="E34" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="6" t="s">
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="J34" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K34" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L34" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="M34" s="6"/>
+      <c r="M34" s="28" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A35" s="36"/>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="48"/>
+      <c r="B35" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="41" t="s">
+      <c r="E35" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="6" t="s">
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="J35" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="K35" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="L35" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="M35" s="6"/>
+      <c r="M35" s="28" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A36" s="36"/>
-      <c r="B36" s="22" t="s">
+      <c r="A36" s="48"/>
+      <c r="B36" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="41" t="s">
+      <c r="E36" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="6" t="s">
         <v>214</v>
       </c>
@@ -2818,30 +2880,30 @@
       <c r="K36" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="M36" s="6"/>
+      <c r="M36" s="57"/>
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A37" s="36"/>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="48"/>
+      <c r="B37" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="41" t="s">
+      <c r="E37" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="6" t="s">
         <v>219</v>
       </c>
@@ -2851,26 +2913,26 @@
       <c r="K37" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="36" t="s">
         <v>217</v>
       </c>
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.15">
-      <c r="A38" s="36"/>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="48"/>
+      <c r="B38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
       <c r="I38" s="6" t="s">
         <v>222</v>
       </c>
@@ -2880,93 +2942,93 @@
       <c r="K38" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="L38" s="36" t="s">
         <v>225</v>
       </c>
       <c r="M38" s="6"/>
     </row>
     <row r="39" spans="1:13" ht="63" x14ac:dyDescent="0.15">
-      <c r="A39" s="37"/>
-      <c r="B39" s="23" t="s">
+      <c r="A39" s="49"/>
+      <c r="B39" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="11" t="s">
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="J39" s="12" t="s">
+      <c r="J39" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="K39" s="11" t="s">
+      <c r="K39" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="L39" s="10" t="s">
+      <c r="L39" s="37" t="s">
         <v>228</v>
       </c>
       <c r="M39" s="6"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="27"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="26"/>
     </row>
     <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="55" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="19" t="s">
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="I41" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="J41" s="21" t="s">
+      <c r="J41" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="K41" s="20" t="s">
+      <c r="K41" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="L41" s="19" t="s">
+      <c r="L41" s="18" t="s">
         <v>238</v>
       </c>
       <c r="M41" s="6"/>
     </row>
     <row r="42" spans="1:13" ht="72" x14ac:dyDescent="0.15">
-      <c r="A42" s="39"/>
-      <c r="B42" s="25" t="s">
+      <c r="A42" s="51"/>
+      <c r="B42" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2987,7 +3049,7 @@
       <c r="H42" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I42" s="26" t="s">
+      <c r="I42" s="25" t="s">
         <v>229</v>
       </c>
       <c r="J42" s="7" t="s">

</xml_diff>

<commit_message>
Agregue el informe, y deje lista la tabla de instrucciones.
</commit_message>
<xml_diff>
--- a/Documentos para el TP final/Tabla de instrucciones.xlsx
+++ b/Documentos para el TP final/Tabla de instrucciones.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="243">
   <si>
     <t>Instrucción</t>
   </si>
@@ -968,7 +968,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,12 +995,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1012,7 +1006,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1072,11 +1066,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1086,26 +1117,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1123,15 +1136,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1144,64 +1148,64 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1211,34 +1215,40 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1545,8 +1555,8 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -1608,1463 +1618,1491 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.15">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="45"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="45"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="45"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="45"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="J6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="45"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="E7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="45"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="30" t="s">
+      <c r="E8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="45"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A10" s="45"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="J10" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="27" t="s">
+      <c r="L10" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="45"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="30" t="s">
+      <c r="E11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="45"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="30" t="s">
+      <c r="E12" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="45"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="30" t="s">
+      <c r="E13" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="45"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="30" t="s">
+      <c r="L14" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="45"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="30" t="s">
+      <c r="E15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A16" s="45"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="E16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="L16" s="30" t="s">
+      <c r="L16" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="M16" s="28" t="s">
+      <c r="M16" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="46"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="37"/>
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="32" t="s">
+      <c r="E17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="34" t="s">
+      <c r="J17" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="K17" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="32" t="s">
+      <c r="L17" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="35" t="s">
+      <c r="M17" s="25" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="26"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="52" t="s">
+      <c r="E19" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="40" t="s">
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="J19" s="41" t="s">
+      <c r="J19" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="M19" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N19" s="43"/>
+      <c r="M19" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N19" s="31"/>
     </row>
     <row r="20" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="48"/>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="49"/>
+      <c r="B20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="53" t="s">
+      <c r="E20" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="28" t="s">
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="L20" s="38" t="s">
+      <c r="L20" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="M20" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N20" s="43"/>
+      <c r="M20" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="48"/>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="49"/>
+      <c r="B21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="53" t="s">
+      <c r="E21" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="28" t="s">
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="M21" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N21" s="43"/>
+      <c r="M21" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N21" s="31"/>
     </row>
     <row r="22" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="48"/>
-      <c r="B22" s="21" t="s">
+      <c r="A22" s="49"/>
+      <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="53" t="s">
+      <c r="E22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="28" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="38" t="s">
+      <c r="L22" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="M22" s="42" t="s">
-        <v>241</v>
-      </c>
-      <c r="N22" s="43"/>
+      <c r="M22" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="N22" s="31"/>
     </row>
     <row r="23" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="48"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="49"/>
+      <c r="B23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="53" t="s">
+      <c r="E23" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="28" t="s">
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="L23" s="38" t="s">
+      <c r="L23" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="M23" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N23" s="43"/>
+      <c r="M23" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N23" s="31"/>
     </row>
     <row r="24" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A24" s="48"/>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="49"/>
+      <c r="B24" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="53" t="s">
+      <c r="E24" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="28" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="28" t="s">
+      <c r="K24" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="L24" s="38" t="s">
+      <c r="L24" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="M24" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N24" s="43"/>
+      <c r="M24" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="48"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="49"/>
+      <c r="B25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="53" t="s">
+      <c r="E25" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="28" t="s">
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="28" t="s">
+      <c r="K25" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="L25" s="38" t="s">
+      <c r="L25" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="M25" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="N25" s="44"/>
+      <c r="M25" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="48"/>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="49"/>
+      <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="53" t="s">
+      <c r="E26" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="28" t="s">
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="K26" s="28" t="s">
+      <c r="K26" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="L26" s="38" t="s">
+      <c r="L26" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A27" s="48"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="49"/>
+      <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="53" t="s">
+      <c r="E27" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="28" t="s">
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K27" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L27" s="38" t="s">
+      <c r="L27" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="M27" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="36" x14ac:dyDescent="0.15">
-      <c r="A28" s="48"/>
-      <c r="B28" s="21" t="s">
+      <c r="A28" s="49"/>
+      <c r="B28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="53" t="s">
+      <c r="E28" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="28" t="s">
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="K28" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="L28" s="38" t="s">
+      <c r="L28" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="M28" s="28" t="s">
+      <c r="M28" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="48"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="49"/>
+      <c r="B29" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="53" t="s">
+      <c r="E29" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="28" t="s">
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="K29" s="28" t="s">
+      <c r="K29" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="L29" s="38" t="s">
+      <c r="L29" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="M29" s="28" t="s">
+      <c r="M29" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="48"/>
-      <c r="B30" s="21" t="s">
+      <c r="A30" s="49"/>
+      <c r="B30" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="53" t="s">
+      <c r="E30" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="28" t="s">
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="L30" s="38" t="s">
+      <c r="L30" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M30" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A31" s="48"/>
-      <c r="B31" s="21" t="s">
+      <c r="A31" s="49"/>
+      <c r="B31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="53" t="s">
+      <c r="E31" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="28" t="s">
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K31" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="L31" s="38" t="s">
+      <c r="L31" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="M31" s="28" t="s">
+      <c r="M31" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="48"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="49"/>
+      <c r="B32" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="53" t="s">
+      <c r="E32" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="28" t="s">
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="J32" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="L32" s="38" t="s">
+      <c r="L32" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="M32" s="28" t="s">
+      <c r="M32" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.15">
-      <c r="A33" s="48"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="49"/>
+      <c r="B33" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="53" t="s">
+      <c r="E33" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="28" t="s">
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="J33" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="K33" s="28" t="s">
+      <c r="K33" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="L33" s="38" t="s">
+      <c r="L33" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="M33" s="28" t="s">
+      <c r="M33" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="36" x14ac:dyDescent="0.15">
-      <c r="A34" s="48"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="49"/>
+      <c r="B34" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="53" t="s">
+      <c r="E34" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="28" t="s">
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="J34" s="29" t="s">
+      <c r="J34" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="K34" s="28" t="s">
+      <c r="K34" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="L34" s="38" t="s">
+      <c r="L34" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="M34" s="28" t="s">
+      <c r="M34" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A35" s="48"/>
-      <c r="B35" s="21" t="s">
+      <c r="A35" s="49"/>
+      <c r="B35" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="53" t="s">
+      <c r="E35" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="28" t="s">
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J35" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="K35" s="28" t="s">
+      <c r="K35" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="L35" s="38" t="s">
+      <c r="L35" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="M35" s="28" t="s">
+      <c r="M35" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A36" s="48"/>
-      <c r="B36" s="21" t="s">
+      <c r="A36" s="49"/>
+      <c r="B36" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="54" t="s">
+      <c r="E36" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="6" t="s">
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="J36" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="L36" s="36" t="s">
+      <c r="L36" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="M36" s="57"/>
+      <c r="M36" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.15">
-      <c r="A37" s="48"/>
-      <c r="B37" s="21" t="s">
+      <c r="A37" s="49"/>
+      <c r="B37" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="54" t="s">
+      <c r="E37" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="6" t="s">
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="K37" s="6" t="s">
+      <c r="K37" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="L37" s="36" t="s">
+      <c r="L37" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="M37" s="6"/>
+      <c r="M37" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.15">
-      <c r="A38" s="48"/>
-      <c r="B38" s="21" t="s">
+      <c r="A38" s="49"/>
+      <c r="B38" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="6" t="s">
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="J38" s="7" t="s">
+      <c r="J38" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="K38" s="6" t="s">
+      <c r="K38" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="L38" s="36" t="s">
+      <c r="L38" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="M38" s="6"/>
+      <c r="M38" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="63" x14ac:dyDescent="0.15">
-      <c r="A39" s="49"/>
-      <c r="B39" s="22" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="56" t="s">
+      <c r="D39" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="10" t="s">
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J39" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K39" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="M39" s="6"/>
+      <c r="M39" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="26"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="16"/>
     </row>
     <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="55" t="s">
+      <c r="E41" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="18" t="s">
+      <c r="F41" s="47"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="I41" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="J41" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="L41" s="18" t="s">
+      <c r="L41" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="M41" s="6"/>
+      <c r="M41" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="72" x14ac:dyDescent="0.15">
-      <c r="A42" s="51"/>
-      <c r="B42" s="24" t="s">
+      <c r="A42" s="40"/>
+      <c r="B42" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="J42" s="7" t="s">
+      <c r="J42" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="K42" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="M42" s="6"/>
+      <c r="M42" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A19:A39"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="D38:H38"/>
@@ -3074,22 +3112,6 @@
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="A19:A39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>